<commit_message>
filling test changed and test2
</commit_message>
<xml_diff>
--- a/tests/ahmad/Filling test results.xlsx
+++ b/tests/ahmad/Filling test results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t xml:space="preserve">Use Case: </t>
   </si>
@@ -75,36 +75,7 @@
 No- The patient not Exist in the DB</t>
   </si>
   <si>
-    <t xml:space="preserve">The patient have HMO approval and referral </t>
-  </si>
-  <si>
-    <t>System throws "Illegible ID" Error Message</t>
-  </si>
-  <si>
-    <t>ID is 9 digits number</t>
-  </si>
-  <si>
     <t>SuccessfulDocumentation</t>
-  </si>
-  <si>
-    <t>IncorrectID</t>
-  </si>
-  <si>
-    <t>Patient has to be enrolled in the system DB Before</t>
-  </si>
-  <si>
-    <t>PatientNotFound</t>
-  </si>
-  <si>
-    <t>1.System throws "Patient not exists in the System" Error Message.
-2. System ask to "Add New Patient"</t>
-  </si>
-  <si>
-    <t>CancelDocumetation</t>
-  </si>
-  <si>
-    <t>System Defines approval in DB
-System shows approval message</t>
   </si>
   <si>
     <t>Filling test results</t>
@@ -129,9 +100,70 @@
     <t xml:space="preserve">type of photos: </t>
   </si>
   <si>
-    <r>
-      <t>Open "Patient Window"
-Type Patient's ID:</t>
+    <t>1.Log in Laboratory worker has logged in
+2.Producing medical test Referral
+3.Viewing Referral info</t>
+  </si>
+  <si>
+    <t>MissingSituationPatient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">situation of patient is empty </t>
+  </si>
+  <si>
+    <t xml:space="preserve">situation of patient can't be only number </t>
+  </si>
+  <si>
+    <t>InvalidSituationPatInt</t>
+  </si>
+  <si>
+    <t>System show "situation of patient  please" Message</t>
+  </si>
+  <si>
+    <t>System show "situation of patient please " Message</t>
+  </si>
+  <si>
+    <t>System show "situation of patient please" Message</t>
+  </si>
+  <si>
+    <t>InvalidSituationPatILess</t>
+  </si>
+  <si>
+    <t>MissingphotoPatILess</t>
+  </si>
+  <si>
+    <t>System show "situation of patient  please attach photos by pressing on "browse.." " Message</t>
+  </si>
+  <si>
+    <t>CancelDocumetation2</t>
+  </si>
+  <si>
+    <t>system throws out warning message "the  test results canceled ".cleaning all fields and return to main window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+System shows approval message</t>
+  </si>
+  <si>
+    <t>Open " test results window" for patient ID: 123456789
+Type situation of patient : 
+Type of photos: "C:\Users\example\photo.jpg "
+Press "submit"</t>
+  </si>
+  <si>
+    <t>attach photos by pressing on "browse.."</t>
+  </si>
+  <si>
+    <t>Open " test results window" for patient ID: 123456789
+Type situation of patient :  situation is normly!, 
+he doesn’t have anything suspecious
+Type photos: "C:\Users\example\photo.jpg "
+Press "submit"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Open " test results window" for patient ID: 123456789
+Type situation of patient : </t>
     </r>
     <r>
       <rPr>
@@ -142,7 +174,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 1234</t>
+      <t>154875</t>
     </r>
     <r>
       <rPr>
@@ -154,102 +186,13 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Press "Enter"
-</t>
-    </r>
-  </si>
-  <si>
-    <t>1.Log in Laboratory worker has logged in
-2.Producing medical test Referral
-3.Viewing Referral info</t>
-  </si>
-  <si>
-    <r>
-      <t>System throws out the warning message"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">patient ID illegal.please insert valid ID </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="177"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"cleaning patient ID field .</t>
-    </r>
-  </si>
-  <si>
-    <t>patient ID can not be char</t>
-  </si>
-  <si>
-    <t>open "patient window"
-type patient ID :
-press "Enter"</t>
-  </si>
-  <si>
-    <r>
-      <t>System throws out the warning message"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">patient ID incorrect.please enter patient ID </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="177"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
-    <t>patient ID is EMPTY</t>
-  </si>
-  <si>
-    <t>MissingPatientID</t>
-  </si>
-  <si>
-    <t>MissingSituationPatient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">situation of patient is empty </t>
-  </si>
-  <si>
-    <t xml:space="preserve">situation of patient can't be only number </t>
-  </si>
-  <si>
-    <t>InvalidSituationPatInt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">situation of patient can't be less than 10 letters </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Open "Patient Window"
-Type Patient's ID: 123456789
-Press "Enter"
-Open " test results window"
+Type photos: "C:\Users\example\photo.jpg "
+Press "submit"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Open " test results window" for patient ID: 123456789
 Type situation of patient :  </t>
     </r>
     <r>
@@ -261,7 +204,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>situa</t>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>situation is normly!, 
+he doesn’t have anything suspecious</t>
     </r>
     <r>
       <rPr>
@@ -273,38 +226,14 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Type of photos: "C:\Users\example\photo.jpg "
+Type  photos: 
 Press "submit"</t>
     </r>
   </si>
   <si>
-    <t>System show "situation of patient  please" Message</t>
-  </si>
-  <si>
-    <t>System show "situation of patient please " Message</t>
-  </si>
-  <si>
-    <t>System show "situation of patient please" Message</t>
-  </si>
-  <si>
-    <t>InvalidSituationPatILess</t>
-  </si>
-  <si>
-    <t>MissingphotoPatILess</t>
-  </si>
-  <si>
-    <t>System show "situation of patient  please attach photos by pressing on "browse.." " Message</t>
-  </si>
-  <si>
-    <t>CancelDocumetation2</t>
-  </si>
-  <si>
-    <t>system throws out warning message "the  test results canceled ".cleaning all fields and return to main window</t>
-  </si>
-  <si>
-    <r>
-      <t>Open "Patient Window"
-Type Patient's ID:</t>
+    <r>
+      <t xml:space="preserve">Open " test results window" for patient ID: 123456789
+Type situation of patient :  </t>
     </r>
     <r>
       <rPr>
@@ -315,17 +244,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">  </t>
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>547854478</t>
+      <t>situation is normly!, 
+he doesn’t have anything suspecious</t>
     </r>
     <r>
       <rPr>
@@ -337,24 +266,28 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Press "Enter"
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>open "patient window"
-type patient ID :</t>
+Type photos: 
+Press "cancle "</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">situation of patient can't be less than 15 letters </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Open " test results window"
+Type situation of patient :  </t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>agba</t>
+      <t>situat</t>
     </r>
     <r>
       <rPr>
@@ -366,154 +299,8 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-press "Enter"</t>
-    </r>
-  </si>
-  <si>
-    <t>Open "Patient Window"
-Type Patient's ID: 123456789
-Press "Cancel"</t>
-  </si>
-  <si>
-    <t>System ask "Do you want to cancle "</t>
-  </si>
-  <si>
-    <t>Open "Patient Window"
-Type Patient's ID: 123456789
-Press "Enter"
-Open " test results window" for patient ID: 123456789
-Type situation of patient :  situation is normly!, 
-he doesn’t have anything suspecious
-attach photos by pressing on "browse.."
-type of photos: "C:\Users\example\photo.jpg "
+Type  photos: "C:\Users\example\photo.jpg "
 Press "submit"</t>
-  </si>
-  <si>
-    <t>Open "Patient Window"
-Type Patient's ID: 123456789
-Press "Enter"
-Open " test results window" for patient ID: 123456789
-Type situation of patient : 
-Type of photos: "C:\Users\example\photo.jpg "
-Press "submit"</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Open "Patient Window"
-Type Patient's ID: 123456789
-Press "Enter"
-Open " test results window" for patient ID: 123456789
-Type situation of patient : </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>154875</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="177"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-type of photos: "C:\Users\example\photo.jpg "
-Press "submit"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Open "Patient Window"
-Type Patient's ID: 123456789
-Press "Enter"
-Open " test results window" for patient ID: 123456789
-Type situation of patient :  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>situation is normly!, 
-he doesn’t have anything suspecious</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="177"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Type of photos: 
-Press "submit"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Open "Patient Window"
-Type Patient's ID: 123456789
-Press "Enter"
-Open " test results window" for patient ID: 123456789
-Type situation of patient :  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>situation is normly!, 
-he doesn’t have anything suspecious</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="177"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Type of photos: 
-Press "cancle "</t>
     </r>
   </si>
 </sst>
@@ -521,7 +308,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -597,20 +384,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -869,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -917,32 +690,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -957,6 +709,21 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1237,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1254,17 +1021,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -1272,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -1285,7 +1052,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -1307,54 +1074,54 @@
       <c r="B8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>32</v>
+      <c r="C8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>123456789</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>31</v>
+      <c r="C9" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>547854478</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
     </row>
     <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
@@ -1370,183 +1137,115 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
-        <v>20</v>
-      </c>
       <c r="B17" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="57.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A19" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="B20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="B21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>58</v>
-      </c>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:4" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="100.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>